<commit_message>
Add photos, PNP (CPL) files and pics
</commit_message>
<xml_diff>
--- a/PCB/BOM_fan_protector.xlsx
+++ b/PCB/BOM_fan_protector.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="BOM_Board1_Schematic1_2023-03-1" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="BOM_Board1_PCB1_2023-03-19" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="36">
   <si>
     <t>No.</t>
   </si>
@@ -43,6 +43,9 @@
     <t>Supplier</t>
   </si>
   <si>
+    <t>Name</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
@@ -100,37 +103,16 @@
     <t>4</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>DEC_TMC?</t>
-  </si>
-  <si>
-    <t>polulu</t>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>R1,R3</t>
+  </si>
+  <si>
+    <t>R0805</t>
   </si>
   <si>
     <t>5</t>
-  </si>
-  <si>
-    <t>H1,H2</t>
-  </si>
-  <si>
-    <t>HDR-TH_4P-P2.54-V-M</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>1K</t>
-  </si>
-  <si>
-    <t>R1,R3</t>
-  </si>
-  <si>
-    <t>R0805</t>
-  </si>
-  <si>
-    <t>7</t>
   </si>
   <si>
     <t>10K</t>
@@ -513,16 +495,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="10" width="20" customWidth="1"/>
+    <col min="1" max="11" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -553,234 +535,188 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>